<commit_message>
almost there!! 1 log_phase characterized
</commit_message>
<xml_diff>
--- a/src/databases/logisticsDB_equipment_python.xlsx
+++ b/src/databases/logisticsDB_equipment_python.xlsx
@@ -1,25 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pchainho\Documents\GitHub\DTOcean-WP5-Installation\src\databases\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="8" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="599" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="599" activeTab="9"/>
   </bookViews>
   <sheets>
-    <sheet name="rov" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="divers" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="cable_burial" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="excavating" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="mattress" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="rock_filter_bags" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="split_pipe" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="hammer" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="drilling_rigs" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="vibro_driver" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="rov" sheetId="1" r:id="rId1"/>
+    <sheet name="divers" sheetId="2" r:id="rId2"/>
+    <sheet name="cable_burial" sheetId="3" r:id="rId3"/>
+    <sheet name="excavating" sheetId="4" r:id="rId4"/>
+    <sheet name="mattress" sheetId="5" r:id="rId5"/>
+    <sheet name="rock_filter_bags" sheetId="6" r:id="rId6"/>
+    <sheet name="split_pipe" sheetId="7" r:id="rId7"/>
+    <sheet name="hammer" sheetId="8" r:id="rId8"/>
+    <sheet name="drilling_rigs" sheetId="9" r:id="rId9"/>
+    <sheet name="vibro_driver" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="152511" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -374,84 +378,67 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="0" numFmtId="165"/>
-    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="12"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="11"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="12"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="000000FF"/>
-      <sz val="11"/>
-      <u val="single"/>
     </font>
   </fonts>
   <fills count="2">
@@ -463,232 +450,483 @@
     </fill>
   </fills>
   <borders count="5">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
-      <right style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thick"/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="thick"/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thick"/>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="thick"/>
-      <bottom style="thick"/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="35">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="3" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="K1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="P12" activeCellId="0" pane="topLeft" sqref="P12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.3921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3137254901961"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7411764705882"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1490196078431"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.721568627451"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1490196078431"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="9.3921568627451"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.4470588235294"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.7490196078431"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.4862745098039"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.5725490196078"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="11.4235294117647"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.4470588235294"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.1686274509804"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.7411764705882"/>
-    <col collapsed="false" hidden="false" max="972" min="23" style="0" width="9.3921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="973" style="0" width="8.63921568627451"/>
+    <col min="1" max="1" width="9.42578125"/>
+    <col min="2" max="2" width="16.85546875"/>
+    <col min="3" max="3" width="14.28515625"/>
+    <col min="4" max="4" width="13.28515625"/>
+    <col min="5" max="5" width="13.7109375"/>
+    <col min="6" max="6" width="13.28515625"/>
+    <col min="7" max="7" width="12.140625"/>
+    <col min="8" max="8" width="12.7109375"/>
+    <col min="9" max="9" width="12.140625"/>
+    <col min="10" max="12" width="9.42578125"/>
+    <col min="13" max="13" width="13.42578125"/>
+    <col min="14" max="14" width="14.7109375"/>
+    <col min="15" max="15" width="16.42578125"/>
+    <col min="16" max="16" width="14.5703125"/>
+    <col min="17" max="17" width="11.5703125"/>
+    <col min="18" max="19" width="11.42578125"/>
+    <col min="20" max="20" width="13.42578125"/>
+    <col min="21" max="21" width="14.140625"/>
+    <col min="22" max="22" width="13.7109375"/>
+    <col min="23" max="972" width="9.42578125"/>
+    <col min="973" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="86.25" outlineLevel="0" r="1">
+    <row r="1" spans="1:33" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -765,312 +1003,311 @@
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="2">
-      <c r="A2" s="4" t="n">
+    <row r="2" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4" t="n">
+      <c r="C2" s="4">
         <v>300</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="4">
         <v>1.8</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="4">
         <v>1.2</v>
       </c>
-      <c r="F2" s="4" t="n">
+      <c r="F2" s="4">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="G2" s="4">
         <v>0.5</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="4" t="n">
+      <c r="I2" s="4">
         <v>100</v>
       </c>
-      <c r="J2" s="4" t="n">
+      <c r="J2" s="4">
         <v>848</v>
       </c>
-      <c r="K2" s="4" t="n">
+      <c r="K2" s="4">
         <v>804</v>
       </c>
-      <c r="L2" s="4" t="n">
+      <c r="L2" s="4">
         <v>760</v>
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
-      <c r="P2" s="4" t="n">
+      <c r="P2" s="4">
         <v>0</v>
       </c>
-      <c r="Q2" s="4" t="n">
+      <c r="Q2" s="4">
         <v>0</v>
       </c>
-      <c r="R2" s="4" t="n">
+      <c r="R2" s="4">
         <v>1</v>
       </c>
-      <c r="S2" s="4" t="n">
+      <c r="S2" s="4">
         <v>1</v>
       </c>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="3">
-      <c r="A3" s="4" t="n">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="7">
         <v>1500</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="7">
         <v>1.5</v>
       </c>
-      <c r="E3" s="7" t="n">
-        <v>0.815</v>
-      </c>
-      <c r="F3" s="7" t="n">
-        <v>0.605</v>
-      </c>
-      <c r="G3" s="7" t="n">
+      <c r="E3" s="7">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="G3" s="7">
         <v>0.2</v>
       </c>
-      <c r="H3" s="7" t="n">
-        <v>0.034</v>
+      <c r="H3" s="7">
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="I3" s="6"/>
-      <c r="J3" s="7" t="n">
+      <c r="J3" s="7">
         <v>66</v>
       </c>
-      <c r="K3" s="7" t="n">
+      <c r="K3" s="7">
         <v>47</v>
       </c>
-      <c r="L3" s="7" t="n">
+      <c r="L3" s="7">
         <v>43</v>
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
-      <c r="P3" s="8" t="n">
+      <c r="P3" s="8">
         <v>29.0671</v>
       </c>
-      <c r="Q3" s="8" t="n">
+      <c r="Q3" s="8">
         <v>27.718</v>
       </c>
-      <c r="R3" s="7" t="n">
+      <c r="R3" s="7">
         <v>1</v>
       </c>
-      <c r="S3" s="7" t="n">
+      <c r="S3" s="7">
         <v>1</v>
       </c>
-      <c r="T3" s="7" t="n">
+      <c r="T3" s="7">
         <v>2300</v>
       </c>
-      <c r="U3" s="7" t="n">
+      <c r="U3" s="7">
         <v>1370</v>
       </c>
-      <c r="V3" s="7" t="n">
+      <c r="V3" s="7">
         <v>1247</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="4">
-      <c r="A4" s="4" t="n">
+    <row r="4" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="4">
         <v>2000</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="4">
         <v>1.4</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="4">
         <v>0.9</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="F4" s="4">
         <v>0.85</v>
       </c>
-      <c r="G4" s="4" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="H4" s="4" t="n">
-        <v>0.045</v>
+      <c r="G4" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H4" s="4">
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="4" t="n">
+      <c r="J4" s="4">
         <v>117</v>
       </c>
-      <c r="K4" s="4" t="n">
+      <c r="K4" s="4">
         <v>88</v>
       </c>
-      <c r="L4" s="4" t="n">
+      <c r="L4" s="4">
         <v>78</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
-      <c r="P4" s="9" t="n">
+      <c r="P4" s="9">
         <v>28.2</v>
       </c>
-      <c r="Q4" s="9" t="n">
+      <c r="Q4" s="9">
         <v>22.5</v>
       </c>
-      <c r="R4" s="4" t="n">
+      <c r="R4" s="4">
         <v>1</v>
       </c>
-      <c r="S4" s="4" t="n">
+      <c r="S4" s="4">
         <v>1</v>
       </c>
-      <c r="T4" s="4" t="n">
+      <c r="T4" s="4">
         <v>2000</v>
       </c>
-      <c r="U4" s="4" t="n">
+      <c r="U4" s="4">
         <v>1900</v>
       </c>
-      <c r="V4" s="4" t="n">
+      <c r="V4" s="4">
         <v>1800</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="5">
-      <c r="A5" s="4" t="n">
+    <row r="5" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4" t="n">
+      <c r="C5" s="4">
         <v>3000</v>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D5" s="4">
         <v>2.59</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="4">
         <v>1.4</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="4">
         <v>1.8</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="4">
         <v>2.54</v>
       </c>
-      <c r="H5" s="4" t="n">
-        <v>0.226</v>
-      </c>
-      <c r="I5" s="4" t="n">
+      <c r="H5" s="4">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="I5" s="4">
         <v>100</v>
       </c>
-      <c r="J5" s="4" t="n">
+      <c r="J5" s="4">
         <v>566</v>
       </c>
-      <c r="K5" s="4" t="n">
+      <c r="K5" s="4">
         <v>537</v>
       </c>
-      <c r="L5" s="4" t="n">
+      <c r="L5" s="4">
         <v>453</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="9" t="n">
+      <c r="P5" s="9">
         <v>82.9</v>
       </c>
-      <c r="Q5" s="9" t="n">
-        <v>66.4</v>
-      </c>
-      <c r="R5" s="4" t="n">
+      <c r="Q5" s="9">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="R5" s="4">
         <v>1</v>
       </c>
-      <c r="S5" s="4" t="n">
+      <c r="S5" s="4">
         <v>2</v>
       </c>
-      <c r="T5" s="4" t="n">
+      <c r="T5" s="4">
         <v>5000</v>
       </c>
-      <c r="U5" s="4" t="n">
+      <c r="U5" s="4">
         <v>1900</v>
       </c>
-      <c r="V5" s="4" t="n">
+      <c r="V5" s="4">
         <v>1800</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="6">
-      <c r="A6" s="4" t="n">
+    <row r="6" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C6" s="4">
         <v>3000</v>
       </c>
-      <c r="D6" s="4" t="n">
-        <v>3.315</v>
-      </c>
-      <c r="E6" s="4" t="n">
+      <c r="D6" s="4">
+        <v>3.3149999999999999</v>
+      </c>
+      <c r="E6" s="4">
         <v>1.73</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="F6" s="4">
         <v>1.73</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="4">
         <v>4.2</v>
       </c>
-      <c r="H6" s="4" t="n">
+      <c r="H6" s="4">
         <v>0.4</v>
       </c>
-      <c r="I6" s="4" t="n">
+      <c r="I6" s="4">
         <v>150</v>
       </c>
-      <c r="J6" s="4" t="n">
+      <c r="J6" s="4">
         <v>800</v>
       </c>
-      <c r="K6" s="4" t="n">
+      <c r="K6" s="4">
         <v>800</v>
       </c>
-      <c r="L6" s="4" t="n">
+      <c r="L6" s="4">
         <v>800</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="9" t="n">
-        <v>67.574</v>
-      </c>
-      <c r="Q6" s="9" t="n">
+      <c r="P6" s="9">
+        <v>67.573999999999998</v>
+      </c>
+      <c r="Q6" s="9">
         <v>69.5</v>
       </c>
-      <c r="R6" s="4" t="n">
+      <c r="R6" s="4">
         <v>1</v>
       </c>
-      <c r="S6" s="4" t="n">
+      <c r="S6" s="4">
         <v>2</v>
       </c>
-      <c r="T6" s="7" t="n">
+      <c r="T6" s="7">
         <v>7000</v>
       </c>
-      <c r="U6" s="7" t="n">
+      <c r="U6" s="7">
         <v>2000</v>
       </c>
-      <c r="V6" s="7" t="n">
-        <f aca="false">1100*4</f>
+      <c r="V6" s="7">
+        <f>1100*4</f>
         <v>4400</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1078,36 +1315,34 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="G1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="M1" activeCellId="0" pane="topLeft" sqref="M1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4745098039216"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9450980392157"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.3137254901961"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="18.8078431372549"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.4862745098039"/>
-    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="13.7411764705882"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.5725490196078"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.8941176470588"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.1686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="9.3921568627451"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="16.85546875"/>
+    <col min="3" max="3" width="16.42578125"/>
+    <col min="4" max="4" width="15.42578125"/>
+    <col min="5" max="5" width="19"/>
+    <col min="6" max="6" width="14.85546875"/>
+    <col min="7" max="7" width="13.28515625"/>
+    <col min="8" max="8" width="14.28515625"/>
+    <col min="9" max="10" width="18.85546875"/>
+    <col min="11" max="11" width="16.42578125"/>
+    <col min="12" max="15" width="13.7109375"/>
+    <col min="16" max="16" width="14.5703125"/>
+    <col min="17" max="17" width="11.5703125"/>
+    <col min="18" max="18" width="14.85546875"/>
+    <col min="19" max="19" width="14.140625"/>
+    <col min="20" max="1025" width="9.42578125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="1">
+    <row r="1" spans="1:20" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -1164,227 +1399,226 @@
         <v>105</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
-      <c r="A2" s="13" t="n">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="n">
-        <v>0.851</v>
-      </c>
-      <c r="C2" s="13" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="D2" s="13" t="n">
-        <v>2.598</v>
-      </c>
-      <c r="E2" s="13" t="n">
+      <c r="B2" s="13">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="C2" s="13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D2" s="13">
+        <v>2.5979999999999999</v>
+      </c>
+      <c r="E2" s="13">
         <v>6.8</v>
       </c>
-      <c r="F2" s="13" t="n">
+      <c r="F2" s="13">
         <v>1.63</v>
       </c>
-      <c r="G2" s="13" t="n">
+      <c r="G2" s="13">
         <v>65</v>
       </c>
-      <c r="H2" s="13" t="n">
+      <c r="H2" s="13">
         <v>26</v>
       </c>
-      <c r="I2" s="13" t="n">
+      <c r="I2" s="13">
         <v>1768</v>
       </c>
-      <c r="J2" s="13" t="n">
+      <c r="J2" s="13">
         <v>600</v>
       </c>
-      <c r="K2" s="13" t="n">
+      <c r="K2" s="13">
         <v>580</v>
       </c>
-      <c r="L2" s="13" t="n">
+      <c r="L2" s="13">
         <v>1734</v>
       </c>
-      <c r="M2" s="13" t="n">
+      <c r="M2" s="13">
         <v>30</v>
       </c>
-      <c r="N2" s="13" t="n">
+      <c r="N2" s="13">
         <v>332</v>
       </c>
-      <c r="O2" s="13" t="n">
+      <c r="O2" s="13">
         <v>554</v>
       </c>
       <c r="P2" s="13"/>
       <c r="Q2" s="13"/>
-      <c r="R2" s="13" t="n">
+      <c r="R2" s="13">
         <v>1000</v>
       </c>
       <c r="S2" s="34"/>
       <c r="T2" s="34"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
-      <c r="A3" s="13" t="n">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="n">
-        <v>1.505</v>
-      </c>
-      <c r="C3" s="13" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="D3" s="13" t="n">
+      <c r="B3" s="13">
+        <v>1.5049999999999999</v>
+      </c>
+      <c r="C3" s="13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D3" s="13">
         <v>3</v>
       </c>
-      <c r="E3" s="13" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="F3" s="13" t="n">
+      <c r="E3" s="13">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F3" s="13">
         <v>5.5</v>
       </c>
-      <c r="G3" s="13" t="n">
+      <c r="G3" s="13">
         <v>120</v>
       </c>
-      <c r="H3" s="13" t="n">
+      <c r="H3" s="13">
         <v>23</v>
       </c>
-      <c r="I3" s="13" t="n">
+      <c r="I3" s="13">
         <v>2555</v>
       </c>
-      <c r="J3" s="13" t="n">
+      <c r="J3" s="13">
         <v>1200</v>
       </c>
-      <c r="K3" s="13" t="n">
+      <c r="K3" s="13">
         <v>740</v>
       </c>
-      <c r="L3" s="13" t="n">
+      <c r="L3" s="13">
         <v>2200</v>
       </c>
-      <c r="M3" s="13" t="n">
+      <c r="M3" s="13">
         <v>80</v>
       </c>
-      <c r="N3" s="13" t="n">
+      <c r="N3" s="13">
         <v>481</v>
       </c>
-      <c r="O3" s="13" t="n">
+      <c r="O3" s="13">
         <v>802</v>
       </c>
       <c r="P3" s="13"/>
       <c r="Q3" s="13"/>
-      <c r="R3" s="13" t="n">
+      <c r="R3" s="13">
         <v>1700</v>
       </c>
       <c r="S3" s="34"/>
       <c r="T3" s="34"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
-      <c r="A4" s="13" t="n">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="n">
+      <c r="B4" s="13">
         <v>2</v>
       </c>
-      <c r="C4" s="13" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="D4" s="13" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="E4" s="13" t="n">
+      <c r="C4" s="13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D4" s="13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E4" s="13">
         <v>19.95</v>
       </c>
-      <c r="F4" s="13" t="n">
+      <c r="F4" s="13">
         <v>10.5</v>
       </c>
-      <c r="G4" s="13" t="n">
+      <c r="G4" s="13">
         <v>265</v>
       </c>
-      <c r="H4" s="13" t="n">
+      <c r="H4" s="13">
         <v>25</v>
       </c>
-      <c r="I4" s="13" t="n">
+      <c r="I4" s="13">
         <v>6666</v>
       </c>
-      <c r="J4" s="13" t="n">
+      <c r="J4" s="13">
         <v>1800</v>
       </c>
-      <c r="K4" s="13" t="n">
+      <c r="K4" s="13">
         <v>1780</v>
       </c>
-      <c r="L4" s="13" t="n">
+      <c r="L4" s="13">
         <v>3600</v>
       </c>
-      <c r="M4" s="13" t="n">
+      <c r="M4" s="13">
         <v>200</v>
       </c>
-      <c r="N4" s="13" t="n">
+      <c r="N4" s="13">
         <v>1376</v>
       </c>
-      <c r="O4" s="13" t="n">
+      <c r="O4" s="13">
         <v>2294</v>
       </c>
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
-      <c r="R4" s="13" t="n">
+      <c r="R4" s="13">
         <v>3500</v>
       </c>
       <c r="S4" s="34"/>
       <c r="T4" s="34"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
-      <c r="A5" s="13" t="n">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="n">
+      <c r="B5" s="13">
         <v>2.25</v>
       </c>
-      <c r="C5" s="13" t="n">
+      <c r="C5" s="13">
         <v>8</v>
       </c>
-      <c r="D5" s="13" t="n">
+      <c r="D5" s="13">
         <v>3.25</v>
       </c>
-      <c r="E5" s="13" t="n">
+      <c r="E5" s="13">
         <v>37</v>
       </c>
-      <c r="F5" s="13" t="n">
+      <c r="F5" s="13">
         <v>10.5</v>
       </c>
-      <c r="G5" s="13" t="n">
+      <c r="G5" s="13">
         <v>400</v>
       </c>
-      <c r="H5" s="13" t="n">
+      <c r="H5" s="13">
         <v>22.5</v>
       </c>
-      <c r="I5" s="13" t="n">
+      <c r="I5" s="13">
         <v>8150</v>
       </c>
-      <c r="J5" s="13" t="n">
+      <c r="J5" s="13">
         <v>4300</v>
       </c>
-      <c r="K5" s="13" t="n">
+      <c r="K5" s="13">
         <v>1500</v>
       </c>
-      <c r="L5" s="13" t="n">
+      <c r="L5" s="13">
         <v>4650</v>
       </c>
-      <c r="M5" s="13" t="n">
+      <c r="M5" s="13">
         <v>300</v>
       </c>
-      <c r="N5" s="13" t="n">
+      <c r="N5" s="13">
         <v>1425</v>
       </c>
-      <c r="O5" s="13" t="n">
+      <c r="O5" s="13">
         <v>1936</v>
       </c>
       <c r="P5" s="13"/>
       <c r="Q5" s="13"/>
-      <c r="R5" s="13" t="n">
+      <c r="R5" s="13">
         <v>5000</v>
       </c>
       <c r="S5" s="34"/>
       <c r="T5" s="34"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1392,33 +1626,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="Q1" activeCellId="0" pane="topLeft" sqref="Q1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5098039215686"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0470588235294"/>
-    <col collapsed="false" hidden="false" max="10" min="6" style="0" width="20.5372549019608"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3294117647059"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.1686274509804"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.7411764705882"/>
-    <col collapsed="false" hidden="false" max="16" min="14" style="0" width="12.5843137254902"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.3137254901961"/>
-    <col collapsed="false" hidden="false" max="1016" min="18" style="0" width="9.3921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.63921568627451"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="16.85546875"/>
+    <col min="3" max="3" width="16.140625"/>
+    <col min="4" max="4" width="18.5703125"/>
+    <col min="5" max="5" width="16"/>
+    <col min="6" max="10" width="20.5703125"/>
+    <col min="11" max="11" width="15.28515625"/>
+    <col min="12" max="12" width="14.140625"/>
+    <col min="13" max="13" width="13.7109375"/>
+    <col min="14" max="16" width="12.5703125"/>
+    <col min="17" max="17" width="14.28515625"/>
+    <col min="18" max="1016" width="9.42578125"/>
+    <col min="1017" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="56.25" outlineLevel="0" r="1">
+    <row r="1" spans="1:17" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>24</v>
@@ -1469,64 +1701,63 @@
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
-      <c r="A2" s="10" t="n">
+    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="11" t="n">
+      <c r="C2" s="11">
         <v>55</v>
       </c>
-      <c r="D2" s="12" t="n">
+      <c r="D2" s="12">
         <v>23.13</v>
       </c>
-      <c r="E2" s="12" t="n">
+      <c r="E2" s="12">
         <v>13.2</v>
       </c>
-      <c r="F2" s="11" t="n">
+      <c r="F2" s="11">
         <v>1</v>
       </c>
-      <c r="G2" s="11" t="n">
+      <c r="G2" s="11">
         <v>2</v>
       </c>
-      <c r="H2" s="11" t="n">
+      <c r="H2" s="11">
         <v>2</v>
       </c>
-      <c r="I2" s="11" t="n">
+      <c r="I2" s="11">
         <v>0</v>
       </c>
-      <c r="J2" s="11" t="n">
+      <c r="J2" s="11">
         <v>0</v>
       </c>
-      <c r="K2" s="11" t="n">
+      <c r="K2" s="11">
         <v>2000</v>
       </c>
-      <c r="L2" s="11" t="n">
+      <c r="L2" s="11">
         <v>800</v>
       </c>
-      <c r="M2" s="11" t="n">
+      <c r="M2" s="11">
         <v>700</v>
       </c>
-      <c r="N2" s="11" t="n">
+      <c r="N2" s="11">
         <v>360</v>
       </c>
-      <c r="O2" s="11" t="n">
+      <c r="O2" s="11">
         <v>520</v>
       </c>
-      <c r="P2" s="11" t="n">
+      <c r="P2" s="11">
         <v>600</v>
       </c>
-      <c r="Q2" s="12" t="n">
+      <c r="Q2" s="12">
         <v>4980</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1534,40 +1765,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E1" activeCellId="0" pane="topLeft" sqref="E1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4862745098039"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7411764705882"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1490196078431"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.721568627451"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1490196078431"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.4235294117647"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.2"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.1490196078431"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.4235294117647"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.7490196078431"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.4862745098039"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.5725490196078"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.4470588235294"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.1686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.63921568627451"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="16.85546875"/>
+    <col min="3" max="3" width="16.42578125"/>
+    <col min="4" max="5" width="13.28515625"/>
+    <col min="6" max="6" width="13.7109375"/>
+    <col min="7" max="7" width="13.28515625"/>
+    <col min="8" max="8" width="12.140625"/>
+    <col min="9" max="9" width="12.7109375"/>
+    <col min="10" max="10" width="12.140625"/>
+    <col min="11" max="11" width="11.42578125"/>
+    <col min="12" max="12" width="16.140625"/>
+    <col min="13" max="13" width="12.140625"/>
+    <col min="14" max="14" width="11.42578125"/>
+    <col min="15" max="15" width="14.7109375"/>
+    <col min="16" max="16" width="16.42578125"/>
+    <col min="17" max="17" width="14.5703125"/>
+    <col min="18" max="18" width="11.5703125"/>
+    <col min="19" max="19" width="13.42578125"/>
+    <col min="20" max="20" width="14.140625"/>
+    <col min="21" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="51" outlineLevel="0" r="1">
+    <row r="1" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>41</v>
@@ -1627,29 +1856,29 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
-      <c r="A2" s="10" t="n">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="11" t="n">
+      <c r="C2" s="11">
         <v>300</v>
       </c>
-      <c r="D2" s="11" t="n">
+      <c r="D2" s="11">
         <v>50</v>
       </c>
-      <c r="E2" s="13" t="n">
+      <c r="E2" s="13">
         <v>9.1</v>
       </c>
-      <c r="F2" s="13" t="n">
+      <c r="F2" s="13">
         <v>4</v>
       </c>
-      <c r="G2" s="13" t="n">
+      <c r="G2" s="13">
         <v>3.5</v>
       </c>
-      <c r="H2" s="13" t="n">
+      <c r="H2" s="13">
         <v>12.2</v>
       </c>
       <c r="I2" s="11" t="s">
@@ -1661,14 +1890,14 @@
       <c r="K2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="11" t="n">
+      <c r="L2" s="11">
         <v>0</v>
       </c>
-      <c r="M2" s="13" t="n">
+      <c r="M2" s="13">
         <v>1.6</v>
       </c>
       <c r="N2" s="11"/>
-      <c r="O2" s="13" t="n">
+      <c r="O2" s="13">
         <v>180</v>
       </c>
       <c r="P2" s="13" t="s">
@@ -1676,34 +1905,34 @@
       </c>
       <c r="Q2" s="13"/>
       <c r="R2" s="13"/>
-      <c r="S2" s="11" t="n">
+      <c r="S2" s="11">
         <v>3600</v>
       </c>
-      <c r="T2" s="11" t="n">
+      <c r="T2" s="11">
         <v>3154</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="3">
-      <c r="A3" s="10" t="n">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="13" t="n">
+      <c r="C3" s="13">
         <v>2500</v>
       </c>
       <c r="D3" s="11"/>
-      <c r="E3" s="13" t="n">
+      <c r="E3" s="13">
         <v>3.1</v>
       </c>
-      <c r="F3" s="13" t="n">
+      <c r="F3" s="13">
         <v>2</v>
       </c>
-      <c r="G3" s="13" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="H3" s="13" t="n">
+      <c r="G3" s="13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H3" s="13">
         <v>6.3</v>
       </c>
       <c r="I3" s="11" t="s">
@@ -1715,46 +1944,46 @@
       <c r="K3" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="11" t="n">
+      <c r="L3" s="11">
         <v>1.5</v>
       </c>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
-      <c r="O3" s="11" t="n">
+      <c r="O3" s="11">
         <v>360</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
-      <c r="S3" s="12" t="n">
+      <c r="S3" s="12">
         <v>4000</v>
       </c>
-      <c r="T3" s="12" t="n">
-        <f aca="false">1100*4</f>
+      <c r="T3" s="12">
+        <f>1100*4</f>
         <v>4400</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="4">
-      <c r="A4" s="10" t="n">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="11" t="n">
+      <c r="C4" s="11">
         <v>1000</v>
       </c>
       <c r="D4" s="11"/>
-      <c r="E4" s="11" t="n">
+      <c r="E4" s="11">
         <v>5</v>
       </c>
-      <c r="F4" s="11" t="n">
-        <v>4.19</v>
-      </c>
-      <c r="G4" s="11" t="n">
+      <c r="F4" s="11">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="G4" s="11">
         <v>2.97</v>
       </c>
-      <c r="H4" s="11" t="n">
+      <c r="H4" s="11">
         <v>13</v>
       </c>
       <c r="I4" s="11" t="s">
@@ -1766,46 +1995,46 @@
       <c r="K4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="11" t="n">
+      <c r="L4" s="11">
         <v>2</v>
       </c>
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
-      <c r="O4" s="11" t="n">
+      <c r="O4" s="11">
         <v>750</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
-      <c r="S4" s="12" t="n">
+      <c r="S4" s="12">
         <v>5000</v>
       </c>
-      <c r="T4" s="12" t="n">
-        <f aca="false">1100*5</f>
+      <c r="T4" s="12">
+        <f>1100*5</f>
         <v>5500</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="5">
-      <c r="A5" s="10" t="n">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="11" t="n">
+      <c r="C5" s="11">
         <v>50</v>
       </c>
       <c r="D5" s="11"/>
-      <c r="E5" s="11" t="n">
+      <c r="E5" s="11">
         <v>7.5</v>
       </c>
-      <c r="F5" s="11" t="n">
+      <c r="F5" s="11">
         <v>7.5</v>
       </c>
-      <c r="G5" s="11" t="n">
+      <c r="G5" s="11">
         <v>4</v>
       </c>
-      <c r="H5" s="11" t="n">
+      <c r="H5" s="11">
         <v>35</v>
       </c>
       <c r="I5" s="11" t="s">
@@ -1817,48 +2046,48 @@
       <c r="K5" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="L5" s="11" t="n">
+      <c r="L5" s="11">
         <v>3</v>
       </c>
       <c r="M5" s="11"/>
-      <c r="N5" s="11" t="n">
+      <c r="N5" s="11">
         <v>1.6</v>
       </c>
-      <c r="O5" s="11" t="n">
+      <c r="O5" s="11">
         <v>550</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
-      <c r="S5" s="12" t="n">
+      <c r="S5" s="12">
         <v>5000</v>
       </c>
-      <c r="T5" s="12" t="n">
+      <c r="T5" s="12">
         <v>10000</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="6">
-      <c r="A6" s="10" t="n">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="11" t="n">
+      <c r="C6" s="11">
         <v>30</v>
       </c>
       <c r="D6" s="11"/>
-      <c r="E6" s="11" t="n">
+      <c r="E6" s="11">
         <v>9</v>
       </c>
-      <c r="F6" s="11" t="n">
+      <c r="F6" s="11">
         <v>4.2</v>
       </c>
-      <c r="G6" s="11" t="n">
+      <c r="G6" s="11">
         <v>2.6</v>
       </c>
-      <c r="H6" s="11" t="n">
-        <v>8.2</v>
+      <c r="H6" s="11">
+        <v>8.1999999999999993</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>55</v>
@@ -1869,17 +2098,17 @@
       <c r="K6" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="L6" s="11" t="n">
-        <v>2.2</v>
+      <c r="L6" s="11">
+        <v>2.2000000000000002</v>
       </c>
       <c r="M6" s="11"/>
-      <c r="N6" s="11" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="O6" s="11" t="n">
+      <c r="N6" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O6" s="11">
         <v>180</v>
       </c>
-      <c r="P6" s="11" t="n">
+      <c r="P6" s="11">
         <v>1.5</v>
       </c>
       <c r="Q6" s="11"/>
@@ -1888,46 +2117,39 @@
       <c r="T6" s="11"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="O1" activeCellId="0" pane="topLeft" sqref="O1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3137254901961"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7411764705882"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7411764705882"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1803921568627"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1490196078431"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.8745098039216"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4352941176471"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.5960784313726"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.4470588235294"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.7490196078431"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.4470588235294"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.1686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.63921568627451"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="14.28515625"/>
+    <col min="3" max="3" width="13.7109375"/>
+    <col min="4" max="4" width="13.28515625"/>
+    <col min="5" max="5" width="13.7109375"/>
+    <col min="6" max="6" width="15.140625"/>
+    <col min="7" max="7" width="12.140625"/>
+    <col min="8" max="8" width="13.85546875"/>
+    <col min="9" max="9" width="12.42578125"/>
+    <col min="10" max="10" width="13.5703125"/>
+    <col min="11" max="11" width="13.42578125"/>
+    <col min="12" max="12" width="14.7109375"/>
+    <col min="13" max="13" width="13.42578125"/>
+    <col min="14" max="14" width="14.140625"/>
+    <col min="15" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="1">
+    <row r="1" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1969,81 +2191,72 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="2">
-      <c r="A2" s="14" t="n">
+    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="n">
+      <c r="B2" s="13">
         <v>300</v>
       </c>
-      <c r="C2" s="13" t="n">
+      <c r="C2" s="13">
         <v>1.8</v>
       </c>
-      <c r="D2" s="13" t="n">
+      <c r="D2" s="13">
         <v>2.8</v>
       </c>
-      <c r="E2" s="13" t="n">
+      <c r="E2" s="13">
         <v>1.7</v>
       </c>
       <c r="F2" s="11"/>
-      <c r="G2" s="13" t="n">
+      <c r="G2" s="13">
         <v>6</v>
       </c>
-      <c r="H2" s="13" t="n">
+      <c r="H2" s="13">
         <v>325</v>
       </c>
-      <c r="I2" s="13" t="n">
+      <c r="I2" s="13">
         <v>400</v>
       </c>
-      <c r="J2" s="13" t="n">
+      <c r="J2" s="13">
         <v>6000</v>
       </c>
-      <c r="K2" s="13" t="n">
+      <c r="K2" s="13">
         <v>3.7</v>
       </c>
-      <c r="L2" s="13" t="n">
+      <c r="L2" s="13">
         <v>270</v>
       </c>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4862745098039"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9058823529412"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.7490196078431"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.721568627451"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1490196078431"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.1686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.63921568627451"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="16.85546875"/>
+    <col min="3" max="3" width="16.42578125"/>
+    <col min="4" max="5" width="13.28515625"/>
+    <col min="6" max="6" width="15.85546875"/>
+    <col min="7" max="7" width="13.28515625"/>
+    <col min="8" max="8" width="14.7109375"/>
+    <col min="9" max="9" width="12.7109375"/>
+    <col min="10" max="10" width="12.140625"/>
+    <col min="11" max="11" width="14.140625"/>
+    <col min="12" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="1">
+    <row r="1" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>67</v>
@@ -2076,147 +2289,138 @@
         <v>76</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
-      <c r="A2" s="15" t="n">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="n">
+      <c r="B2" s="15">
         <v>37</v>
       </c>
-      <c r="C2" s="15" t="n">
+      <c r="C2" s="15">
         <v>2400</v>
       </c>
-      <c r="D2" s="16" t="n">
+      <c r="D2" s="16">
         <v>5.99</v>
       </c>
-      <c r="E2" s="15" t="n">
+      <c r="E2" s="15">
         <v>2.99</v>
       </c>
-      <c r="F2" s="17" t="n">
+      <c r="F2" s="17">
         <v>0.15</v>
       </c>
-      <c r="G2" s="15" t="n">
+      <c r="G2" s="15">
         <v>5.13</v>
       </c>
-      <c r="H2" s="15" t="n">
+      <c r="H2" s="15">
         <v>2.94</v>
       </c>
-      <c r="I2" s="15" t="n">
+      <c r="I2" s="15">
         <v>12</v>
       </c>
-      <c r="J2" s="15" t="n">
+      <c r="J2" s="15">
         <v>16</v>
       </c>
-      <c r="K2" s="15" t="n">
+      <c r="K2" s="15">
         <v>627</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
-      <c r="A3" s="18" t="n">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="n">
+      <c r="B3" s="18">
         <v>37</v>
       </c>
-      <c r="C3" s="18" t="n">
+      <c r="C3" s="18">
         <v>2400</v>
       </c>
-      <c r="D3" s="18" t="n">
+      <c r="D3" s="18">
         <v>5.984</v>
       </c>
-      <c r="E3" s="18" t="n">
-        <v>2.979</v>
-      </c>
-      <c r="F3" s="18" t="n">
+      <c r="E3" s="18">
+        <v>2.9790000000000001</v>
+      </c>
+      <c r="F3" s="18">
         <v>0.3</v>
       </c>
-      <c r="G3" s="18" t="n">
+      <c r="G3" s="18">
         <v>9.1</v>
       </c>
-      <c r="H3" s="18" t="n">
+      <c r="H3" s="18">
         <v>5.2</v>
       </c>
-      <c r="I3" s="18" t="n">
+      <c r="I3" s="18">
         <v>10</v>
       </c>
-      <c r="J3" s="18" t="n">
+      <c r="J3" s="18">
         <v>20</v>
       </c>
-      <c r="K3" s="18" t="n">
+      <c r="K3" s="18">
         <v>955</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
-      <c r="A4" s="13" t="n">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="n">
+      <c r="B4" s="13">
         <v>37</v>
       </c>
-      <c r="C4" s="13" t="n">
+      <c r="C4" s="13">
         <v>2400</v>
       </c>
-      <c r="D4" s="13" t="n">
+      <c r="D4" s="13">
         <v>5.97</v>
       </c>
-      <c r="E4" s="13" t="n">
+      <c r="E4" s="13">
         <v>2.99</v>
       </c>
-      <c r="F4" s="13" t="n">
+      <c r="F4" s="13">
         <v>0.45</v>
       </c>
-      <c r="G4" s="13" t="n">
+      <c r="G4" s="13">
         <v>11.78</v>
       </c>
-      <c r="H4" s="13" t="n">
+      <c r="H4" s="13">
         <v>6.75</v>
       </c>
-      <c r="I4" s="13" t="n">
+      <c r="I4" s="13">
         <v>7</v>
       </c>
-      <c r="J4" s="13" t="n">
+      <c r="J4" s="13">
         <v>32</v>
       </c>
-      <c r="K4" s="13" t="n">
+      <c r="K4" s="13">
         <v>2090</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4862745098039"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9058823529412"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.7490196078431"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8705882352941"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.1686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.63921568627451"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="16.85546875"/>
+    <col min="3" max="3" width="16.42578125"/>
+    <col min="4" max="5" width="13.28515625"/>
+    <col min="6" max="6" width="15.85546875"/>
+    <col min="7" max="7" width="13.28515625"/>
+    <col min="8" max="8" width="14.7109375"/>
+    <col min="9" max="9" width="12.85546875"/>
+    <col min="10" max="10" width="14.140625"/>
+    <col min="11" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="1">
+    <row r="1" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>5</v>
@@ -2246,7 +2450,7 @@
         <v>76</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -2258,7 +2462,7 @@
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -2270,7 +2474,7 @@
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -2283,40 +2487,33 @@
       <c r="J4" s="13"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E2" activeCellId="0" pane="topLeft" sqref="E2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4862745098039"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9058823529412"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="14.7490196078431"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.1686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.63921568627451"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="16.85546875"/>
+    <col min="3" max="3" width="16.42578125"/>
+    <col min="4" max="5" width="13.28515625"/>
+    <col min="6" max="6" width="15.85546875"/>
+    <col min="7" max="7" width="13.28515625"/>
+    <col min="8" max="10" width="14.7109375"/>
+    <col min="11" max="11" width="14.140625"/>
+    <col min="12" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="1">
+    <row r="1" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>83</v>
@@ -2349,7 +2546,7 @@
         <v>76</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -2362,7 +2559,7 @@
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -2375,7 +2572,7 @@
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -2389,45 +2586,38 @@
       <c r="K4" s="13"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4745098039216"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.4862745098039"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7411764705882"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1490196078431"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8078431372549"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.5725490196078"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.8941176470588"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.1686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.63921568627451"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="16.85546875"/>
+    <col min="3" max="3" width="16.42578125"/>
+    <col min="4" max="4" width="15.42578125"/>
+    <col min="5" max="5" width="16.42578125"/>
+    <col min="6" max="6" width="13.7109375"/>
+    <col min="7" max="7" width="13.28515625"/>
+    <col min="8" max="8" width="12.140625"/>
+    <col min="9" max="9" width="18.85546875"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875"/>
+    <col min="13" max="13" width="14.140625"/>
+    <col min="14" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="1">
+    <row r="1" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2466,80 +2656,73 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
-      <c r="A2" s="19" t="n">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="19" t="n">
+      <c r="C2" s="19">
         <v>22.1</v>
       </c>
-      <c r="D2" s="19" t="n">
+      <c r="D2" s="19">
         <v>217.5</v>
       </c>
-      <c r="E2" s="19" t="n">
+      <c r="E2" s="19">
         <v>3.75</v>
       </c>
-      <c r="F2" s="19" t="n">
+      <c r="F2" s="19">
         <v>4.74</v>
       </c>
-      <c r="G2" s="20" t="n">
+      <c r="G2" s="20">
         <v>1900</v>
       </c>
-      <c r="H2" s="20" t="n">
+      <c r="H2" s="20">
         <v>190</v>
       </c>
-      <c r="I2" s="20" t="n">
+      <c r="I2" s="20">
         <v>32</v>
       </c>
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
-      <c r="L2" s="21" t="n">
+      <c r="L2" s="21">
         <v>18400</v>
       </c>
       <c r="M2" s="22"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AB2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMI2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G1" activeCellId="0" pane="topLeft" sqref="G1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="16.4862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="15.4745098039216"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="18.9450980392157"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="13.7411764705882"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="23" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="23" width="12.1490196078431"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="23" width="18.8078431372549"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="23" width="14.6"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="23" width="11.5725490196078"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="23" width="14.8941176470588"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="23" width="14.1686274509804"/>
-    <col collapsed="false" hidden="false" max="1023" min="14" style="23" width="8.67843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.63921568627451"/>
+    <col min="1" max="1" width="9.28515625" style="23"/>
+    <col min="2" max="2" width="16.85546875" style="23"/>
+    <col min="3" max="3" width="16.42578125" style="23"/>
+    <col min="4" max="4" width="15.42578125" style="23"/>
+    <col min="5" max="5" width="19" style="23"/>
+    <col min="6" max="6" width="13.7109375" style="23"/>
+    <col min="7" max="7" width="13.28515625" style="23"/>
+    <col min="8" max="8" width="12.140625" style="23"/>
+    <col min="9" max="9" width="18.85546875" style="23"/>
+    <col min="10" max="10" width="14.5703125" style="23"/>
+    <col min="11" max="11" width="11.5703125" style="23"/>
+    <col min="12" max="12" width="14.85546875" style="23"/>
+    <col min="13" max="13" width="14.140625" style="23"/>
+    <col min="14" max="1023" width="8.7109375" style="23"/>
+    <col min="1024" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="52.5" outlineLevel="0" r="1">
+    <row r="1" spans="1:28" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
       <c r="B1" s="2" t="s">
         <v>79</v>
@@ -2593,37 +2776,37 @@
       <c r="AA1" s="24"/>
       <c r="AB1" s="24"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
-      <c r="A2" s="12" t="n">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="n">
+      <c r="B2" s="12">
         <v>5</v>
       </c>
-      <c r="C2" s="12" t="n">
+      <c r="C2" s="12">
         <v>11.53</v>
       </c>
-      <c r="D2" s="12" t="n">
+      <c r="D2" s="12">
         <v>65</v>
       </c>
-      <c r="E2" s="12" t="n">
+      <c r="E2" s="12">
         <v>6</v>
       </c>
-      <c r="F2" s="26" t="n">
+      <c r="F2" s="26">
         <v>70</v>
       </c>
-      <c r="G2" s="26" t="n">
+      <c r="G2" s="26">
         <v>30</v>
       </c>
-      <c r="H2" s="12" t="n">
+      <c r="H2" s="12">
         <v>393</v>
       </c>
-      <c r="I2" s="12" t="n">
+      <c r="I2" s="12">
         <v>250</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
-      <c r="L2" s="27" t="n">
+      <c r="L2" s="27">
         <v>240000</v>
       </c>
       <c r="M2" s="28"/>
@@ -2644,12 +2827,7 @@
       <c r="AB2" s="29"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
yeah yeah YEAH! Matching up and running!!!! =)
</commit_message>
<xml_diff>
--- a/src/databases/logisticsDB_equipment_python.xlsx
+++ b/src/databases/logisticsDB_equipment_python.xlsx
@@ -1,29 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pchainho\Documents\GitHub\DTOcean-WP5-Installation\src\databases\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="599" firstSheet="3" activeTab="9"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="599" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="rov" sheetId="1" r:id="rId1"/>
-    <sheet name="divers" sheetId="2" r:id="rId2"/>
-    <sheet name="cable_burial" sheetId="3" r:id="rId3"/>
-    <sheet name="excavating" sheetId="4" r:id="rId4"/>
-    <sheet name="mattress" sheetId="5" r:id="rId5"/>
-    <sheet name="rock_filter_bags" sheetId="6" r:id="rId6"/>
-    <sheet name="split_pipe" sheetId="7" r:id="rId7"/>
-    <sheet name="hammer" sheetId="8" r:id="rId8"/>
-    <sheet name="drilling_rigs" sheetId="9" r:id="rId9"/>
-    <sheet name="vibro_driver" sheetId="10" r:id="rId10"/>
+    <sheet name="rov" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="divers" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="cable_burial" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="excavating" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="mattress" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="rock_filter_bags" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="split_pipe" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="hammer" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="drilling_rigs" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="vibro_driver" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="152511" calcOnSave="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
@@ -378,67 +374,84 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="0" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="00000000"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
-      <charset val="1"/>
+      <sz val="12"/>
     </font>
     <font>
-      <u/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <color rgb="00000000"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+    </font>
+    <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
+      <b val="true"/>
+      <color rgb="00000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <charset val="1"/>
+      <family val="2"/>
+      <color rgb="000000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
     </font>
   </fonts>
   <fills count="2">
@@ -450,483 +463,232 @@
     </fill>
   </fills>
   <borders count="5">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="thick"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="thick"/>
+      <right style="thick"/>
       <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="thick"/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="thick"/>
       <right/>
       <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="thick"/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="thick"/>
       <right/>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
+      <top style="thick"/>
+      <bottom style="thick"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="35">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="5" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="3" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B11" activeCellId="0" pane="topLeft" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125"/>
-    <col min="2" max="2" width="16.85546875"/>
-    <col min="3" max="3" width="14.28515625"/>
-    <col min="4" max="4" width="13.28515625"/>
-    <col min="5" max="5" width="13.7109375"/>
-    <col min="6" max="6" width="13.28515625"/>
-    <col min="7" max="7" width="12.140625"/>
-    <col min="8" max="8" width="12.7109375"/>
-    <col min="9" max="9" width="12.140625"/>
-    <col min="10" max="12" width="9.42578125"/>
-    <col min="13" max="13" width="13.42578125"/>
-    <col min="14" max="14" width="14.7109375"/>
-    <col min="15" max="15" width="16.42578125"/>
-    <col min="16" max="16" width="14.5703125"/>
-    <col min="17" max="17" width="11.5703125"/>
-    <col min="18" max="19" width="11.42578125"/>
-    <col min="20" max="20" width="13.42578125"/>
-    <col min="21" max="21" width="14.140625"/>
-    <col min="22" max="22" width="13.7109375"/>
-    <col min="23" max="972" width="9.42578125"/>
-    <col min="973" max="1025" width="8.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.46666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3411764705882"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7686274509804"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1921568627451"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.7647058823529"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="9.46666666666667"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.4823529411765"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.7725490196078"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.6274509803922"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="11.4745098039216"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.4823529411765"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.2"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.7686274509804"/>
+    <col collapsed="false" hidden="false" max="972" min="23" style="0" width="9.46666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="973" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="86.25" outlineLevel="0" r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1003,311 +765,312 @@
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
     </row>
-    <row r="2" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="2">
+      <c r="A2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="4" t="n">
         <v>300</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="4" t="n">
         <v>1.8</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="4" t="n">
         <v>1.2</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="4" t="n">
         <v>0.5</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="4" t="n">
         <v>848</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="4" t="n">
         <v>804</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="4" t="n">
         <v>760</v>
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
-      <c r="P2" s="4">
+      <c r="P2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R2" s="4">
+      <c r="R2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="S2" s="4">
+      <c r="S2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="3">
+      <c r="A3" s="4" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="7" t="n">
         <v>1500</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="7" t="n">
         <v>1.5</v>
       </c>
-      <c r="E3" s="7">
-        <v>0.81499999999999995</v>
-      </c>
-      <c r="F3" s="7">
-        <v>0.60499999999999998</v>
-      </c>
-      <c r="G3" s="7">
+      <c r="E3" s="7" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="F3" s="7" t="n">
+        <v>0.605</v>
+      </c>
+      <c r="G3" s="7" t="n">
         <v>0.2</v>
       </c>
-      <c r="H3" s="7">
-        <v>3.4000000000000002E-2</v>
+      <c r="H3" s="7" t="n">
+        <v>0.034</v>
       </c>
       <c r="I3" s="6"/>
-      <c r="J3" s="7">
+      <c r="J3" s="7" t="n">
         <v>66</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="7" t="n">
         <v>47</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="7" t="n">
         <v>43</v>
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
-      <c r="P3" s="8">
+      <c r="P3" s="8" t="n">
         <v>29.0671</v>
       </c>
-      <c r="Q3" s="8">
+      <c r="Q3" s="8" t="n">
         <v>27.718</v>
       </c>
-      <c r="R3" s="7">
+      <c r="R3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="S3" s="7">
+      <c r="S3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="T3" s="7">
+      <c r="T3" s="7" t="n">
         <v>2300</v>
       </c>
-      <c r="U3" s="7">
+      <c r="U3" s="7" t="n">
         <v>1370</v>
       </c>
-      <c r="V3" s="7">
+      <c r="V3" s="7" t="n">
         <v>1247</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="4">
+      <c r="A4" s="4" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="4" t="n">
         <v>2000</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="4" t="n">
         <v>1.4</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="4" t="n">
         <v>0.9</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="4" t="n">
         <v>0.85</v>
       </c>
-      <c r="G4" s="4">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="H4" s="4">
-        <v>4.4999999999999998E-2</v>
+      <c r="G4" s="4" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>0.045</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="4">
+      <c r="J4" s="4" t="n">
         <v>117</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="4" t="n">
         <v>88</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="4" t="n">
         <v>78</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
-      <c r="P4" s="9">
+      <c r="P4" s="9" t="n">
         <v>28.2</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="Q4" s="9" t="n">
         <v>22.5</v>
       </c>
-      <c r="R4" s="4">
+      <c r="R4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="S4" s="4">
+      <c r="S4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="T4" s="4">
+      <c r="T4" s="4" t="n">
         <v>2000</v>
       </c>
-      <c r="U4" s="4">
+      <c r="U4" s="4" t="n">
         <v>1900</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4" s="4" t="n">
         <v>1800</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="5">
+      <c r="A5" s="4" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="4" t="n">
         <v>3000</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="4" t="n">
         <v>2.59</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="4" t="n">
         <v>1.4</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="4" t="n">
         <v>1.8</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="4" t="n">
         <v>2.54</v>
       </c>
-      <c r="H5" s="4">
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="I5" s="4">
+      <c r="H5" s="4" t="n">
+        <v>0.226</v>
+      </c>
+      <c r="I5" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="4" t="n">
         <v>566</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="4" t="n">
         <v>537</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="4" t="n">
         <v>453</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="9">
+      <c r="P5" s="9" t="n">
         <v>82.9</v>
       </c>
-      <c r="Q5" s="9">
-        <v>66.400000000000006</v>
-      </c>
-      <c r="R5" s="4">
+      <c r="Q5" s="9" t="n">
+        <v>66.4</v>
+      </c>
+      <c r="R5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="T5" s="4">
+      <c r="T5" s="4" t="n">
         <v>5000</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U5" s="4" t="n">
         <v>1900</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V5" s="4" t="n">
         <v>1800</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="6">
+      <c r="A6" s="4" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="4" t="n">
         <v>3000</v>
       </c>
-      <c r="D6" s="4">
-        <v>3.3149999999999999</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="D6" s="4" t="n">
+        <v>3.315</v>
+      </c>
+      <c r="E6" s="4" t="n">
         <v>1.73</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="4" t="n">
         <v>1.73</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="4" t="n">
         <v>4.2</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="4" t="n">
         <v>0.4</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="4" t="n">
         <v>150</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="4" t="n">
         <v>800</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="4" t="n">
         <v>800</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="4" t="n">
         <v>800</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="9">
-        <v>67.573999999999998</v>
-      </c>
-      <c r="Q6" s="9">
+      <c r="P6" s="9" t="n">
+        <v>67.574</v>
+      </c>
+      <c r="Q6" s="9" t="n">
         <v>69.5</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="S6" s="4">
+      <c r="S6" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="T6" s="7">
+      <c r="T6" s="7" t="n">
         <v>7000</v>
       </c>
-      <c r="U6" s="7">
+      <c r="U6" s="7" t="n">
         <v>2000</v>
       </c>
-      <c r="V6" s="7">
-        <f>1100*4</f>
+      <c r="V6" s="7" t="n">
+        <f aca="false">1100*4</f>
         <v>4400</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1315,34 +1078,36 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="H21" activeCellId="0" pane="topLeft" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125"/>
-    <col min="2" max="2" width="16.85546875"/>
-    <col min="3" max="3" width="16.42578125"/>
-    <col min="4" max="4" width="15.42578125"/>
-    <col min="5" max="5" width="19"/>
-    <col min="6" max="6" width="14.85546875"/>
-    <col min="7" max="7" width="13.28515625"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="10" width="18.85546875"/>
-    <col min="11" max="11" width="16.42578125"/>
-    <col min="12" max="15" width="13.7109375"/>
-    <col min="16" max="16" width="14.5703125"/>
-    <col min="17" max="17" width="11.5703125"/>
-    <col min="18" max="18" width="14.85546875"/>
-    <col min="19" max="19" width="14.140625"/>
-    <col min="20" max="1025" width="9.42578125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4901960784314"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.0823529411765"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.9137254901961"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9176470588235"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="18.9294117647059"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="13.7686274509804"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.6274509803922"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.9137254901961"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="9.46666666666667"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="47.25" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -1399,226 +1164,227 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+      <c r="A2" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="13">
-        <v>0.85099999999999998</v>
-      </c>
-      <c r="C2" s="13">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D2" s="13">
-        <v>2.5979999999999999</v>
-      </c>
-      <c r="E2" s="13">
+      <c r="B2" s="13" t="n">
+        <v>0.851</v>
+      </c>
+      <c r="C2" s="13" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D2" s="13" t="n">
+        <v>2.598</v>
+      </c>
+      <c r="E2" s="13" t="n">
         <v>6.8</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="13" t="n">
         <v>1.63</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="13" t="n">
         <v>65</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="13" t="n">
         <v>26</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="13" t="n">
         <v>1768</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="13" t="n">
         <v>600</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="13" t="n">
         <v>580</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="13" t="n">
         <v>1734</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="13" t="n">
         <v>30</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="13" t="n">
         <v>332</v>
       </c>
-      <c r="O2" s="13">
+      <c r="O2" s="13" t="n">
         <v>554</v>
       </c>
       <c r="P2" s="13"/>
       <c r="Q2" s="13"/>
-      <c r="R2" s="13">
+      <c r="R2" s="13" t="n">
         <v>1000</v>
       </c>
       <c r="S2" s="34"/>
       <c r="T2" s="34"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+      <c r="A3" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="13">
-        <v>1.5049999999999999</v>
-      </c>
-      <c r="C3" s="13">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D3" s="13">
+      <c r="B3" s="13" t="n">
+        <v>1.505</v>
+      </c>
+      <c r="C3" s="13" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D3" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="E3" s="13">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="F3" s="13">
+      <c r="E3" s="13" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="F3" s="13" t="n">
         <v>5.5</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="13" t="n">
         <v>120</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="13" t="n">
         <v>23</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="13" t="n">
         <v>2555</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="13" t="n">
         <v>1200</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="13" t="n">
         <v>740</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L3" s="13" t="n">
         <v>2200</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="13" t="n">
         <v>80</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="13" t="n">
         <v>481</v>
       </c>
-      <c r="O3" s="13">
+      <c r="O3" s="13" t="n">
         <v>802</v>
       </c>
       <c r="P3" s="13"/>
       <c r="Q3" s="13"/>
-      <c r="R3" s="13">
+      <c r="R3" s="13" t="n">
         <v>1700</v>
       </c>
       <c r="S3" s="34"/>
       <c r="T3" s="34"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+      <c r="A4" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="13">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D4" s="13">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E4" s="13">
+      <c r="C4" s="13" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="D4" s="13" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E4" s="13" t="n">
         <v>19.95</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="13" t="n">
         <v>10.5</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="13" t="n">
         <v>265</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="13" t="n">
         <v>25</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="13" t="n">
         <v>6666</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="13" t="n">
         <v>1800</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="13" t="n">
         <v>1780</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="13" t="n">
         <v>3600</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="13" t="n">
         <v>200</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="13" t="n">
         <v>1376</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="13" t="n">
         <v>2294</v>
       </c>
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
-      <c r="R4" s="13">
+      <c r="R4" s="13" t="n">
         <v>3500</v>
       </c>
       <c r="S4" s="34"/>
       <c r="T4" s="34"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+      <c r="A5" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="13" t="n">
         <v>2.25</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="13" t="n">
         <v>3.25</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="13" t="n">
         <v>37</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="13" t="n">
         <v>10.5</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="13" t="n">
         <v>400</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="13" t="n">
         <v>22.5</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="13" t="n">
         <v>8150</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="13" t="n">
         <v>4300</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="13" t="n">
         <v>1500</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="13" t="n">
         <v>4650</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="13" t="n">
         <v>300</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="13" t="n">
         <v>1425</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="13" t="n">
         <v>1936</v>
       </c>
       <c r="P5" s="13"/>
       <c r="Q5" s="13"/>
-      <c r="R5" s="13">
+      <c r="R5" s="13" t="n">
         <v>5000</v>
       </c>
       <c r="S5" s="34"/>
       <c r="T5" s="34"/>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1626,31 +1392,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125"/>
-    <col min="2" max="2" width="16.85546875"/>
-    <col min="3" max="3" width="16.140625"/>
-    <col min="4" max="4" width="18.5703125"/>
-    <col min="5" max="5" width="16"/>
-    <col min="6" max="10" width="20.5703125"/>
-    <col min="11" max="11" width="15.28515625"/>
-    <col min="12" max="12" width="14.140625"/>
-    <col min="13" max="13" width="13.7109375"/>
-    <col min="14" max="16" width="12.5703125"/>
-    <col min="17" max="17" width="14.28515625"/>
-    <col min="18" max="1016" width="9.42578125"/>
-    <col min="1017" max="1025" width="8.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2078431372549"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0705882352941"/>
+    <col collapsed="false" hidden="false" max="10" min="6" style="0" width="20.6588235294118"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3450980392157"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.2"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.7686274509804"/>
+    <col collapsed="false" hidden="false" max="16" min="14" style="0" width="12.6196078431373"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.3411764705882"/>
+    <col collapsed="false" hidden="false" max="1016" min="18" style="0" width="9.46666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="56.25" outlineLevel="0" r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>24</v>
@@ -1701,63 +1469,64 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
+      <c r="A2" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="11" t="n">
         <v>55</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="12" t="n">
         <v>23.13</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="12" t="n">
         <v>13.2</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="11" t="n">
         <v>2000</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="11" t="n">
         <v>800</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="11" t="n">
         <v>700</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="11" t="n">
         <v>360</v>
       </c>
-      <c r="O2" s="11">
+      <c r="O2" s="11" t="n">
         <v>520</v>
       </c>
-      <c r="P2" s="11">
+      <c r="P2" s="11" t="n">
         <v>600</v>
       </c>
-      <c r="Q2" s="12">
+      <c r="Q2" s="12" t="n">
         <v>4980</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1765,38 +1534,40 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E1" activeCellId="0" pane="topLeft" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125"/>
-    <col min="2" max="2" width="16.85546875"/>
-    <col min="3" max="3" width="16.42578125"/>
-    <col min="4" max="5" width="13.28515625"/>
-    <col min="6" max="6" width="13.7109375"/>
-    <col min="7" max="7" width="13.28515625"/>
-    <col min="8" max="8" width="12.140625"/>
-    <col min="9" max="9" width="12.7109375"/>
-    <col min="10" max="10" width="12.140625"/>
-    <col min="11" max="11" width="11.42578125"/>
-    <col min="12" max="12" width="16.140625"/>
-    <col min="13" max="13" width="12.140625"/>
-    <col min="14" max="14" width="11.42578125"/>
-    <col min="15" max="15" width="14.7109375"/>
-    <col min="16" max="16" width="16.42578125"/>
-    <col min="17" max="17" width="14.5703125"/>
-    <col min="18" max="18" width="11.5703125"/>
-    <col min="19" max="19" width="13.42578125"/>
-    <col min="20" max="20" width="14.140625"/>
-    <col min="21" max="1025" width="8.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7686274509804"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1921568627451"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.7647058823529"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1921568627451"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.4745098039216"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.2078431372549"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.1921568627451"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.4745098039216"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.7725490196078"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.6274509803922"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.4823529411765"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="51" outlineLevel="0" r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>41</v>
@@ -1856,29 +1627,29 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
+      <c r="A2" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="11" t="n">
         <v>300</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="13" t="n">
         <v>9.1</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="13" t="n">
         <v>3.5</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="13" t="n">
         <v>12.2</v>
       </c>
       <c r="I2" s="11" t="s">
@@ -1890,14 +1661,14 @@
       <c r="K2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="13" t="n">
         <v>1.6</v>
       </c>
       <c r="N2" s="11"/>
-      <c r="O2" s="13">
+      <c r="O2" s="13" t="n">
         <v>180</v>
       </c>
       <c r="P2" s="13" t="s">
@@ -1905,34 +1676,34 @@
       </c>
       <c r="Q2" s="13"/>
       <c r="R2" s="13"/>
-      <c r="S2" s="11">
+      <c r="S2" s="11" t="n">
         <v>3600</v>
       </c>
-      <c r="T2" s="11">
+      <c r="T2" s="11" t="n">
         <v>3154</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="3">
+      <c r="A3" s="10" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="13" t="n">
         <v>2500</v>
       </c>
       <c r="D3" s="11"/>
-      <c r="E3" s="13">
+      <c r="E3" s="13" t="n">
         <v>3.1</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="13">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H3" s="13">
+      <c r="G3" s="13" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H3" s="13" t="n">
         <v>6.3</v>
       </c>
       <c r="I3" s="11" t="s">
@@ -1944,46 +1715,46 @@
       <c r="K3" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="11" t="n">
         <v>1.5</v>
       </c>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
-      <c r="O3" s="11">
+      <c r="O3" s="11" t="n">
         <v>360</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
-      <c r="S3" s="12">
+      <c r="S3" s="12" t="n">
         <v>4000</v>
       </c>
-      <c r="T3" s="12">
-        <f>1100*4</f>
+      <c r="T3" s="12" t="n">
+        <f aca="false">1100*4</f>
         <v>4400</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="4">
+      <c r="A4" s="10" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="11" t="n">
         <v>1000</v>
       </c>
       <c r="D4" s="11"/>
-      <c r="E4" s="11">
+      <c r="E4" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="F4" s="11">
-        <v>4.1900000000000004</v>
-      </c>
-      <c r="G4" s="11">
+      <c r="F4" s="11" t="n">
+        <v>4.19</v>
+      </c>
+      <c r="G4" s="11" t="n">
         <v>2.97</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="11" t="n">
         <v>13</v>
       </c>
       <c r="I4" s="11" t="s">
@@ -1995,46 +1766,46 @@
       <c r="K4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="11" t="n">
         <v>2</v>
       </c>
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
-      <c r="O4" s="11">
+      <c r="O4" s="11" t="n">
         <v>750</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
-      <c r="S4" s="12">
+      <c r="S4" s="12" t="n">
         <v>5000</v>
       </c>
-      <c r="T4" s="12">
-        <f>1100*5</f>
+      <c r="T4" s="12" t="n">
+        <f aca="false">1100*5</f>
         <v>5500</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="5">
+      <c r="A5" s="10" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="11" t="n">
         <v>50</v>
       </c>
       <c r="D5" s="11"/>
-      <c r="E5" s="11">
+      <c r="E5" s="11" t="n">
         <v>7.5</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="11" t="n">
         <v>7.5</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="11" t="n">
         <v>35</v>
       </c>
       <c r="I5" s="11" t="s">
@@ -2046,48 +1817,48 @@
       <c r="K5" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="11" t="n">
         <v>3</v>
       </c>
       <c r="M5" s="11"/>
-      <c r="N5" s="11">
+      <c r="N5" s="11" t="n">
         <v>1.6</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="11" t="n">
         <v>550</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
-      <c r="S5" s="12">
+      <c r="S5" s="12" t="n">
         <v>5000</v>
       </c>
-      <c r="T5" s="12">
+      <c r="T5" s="12" t="n">
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="6">
+      <c r="A6" s="10" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="11" t="n">
         <v>30</v>
       </c>
       <c r="D6" s="11"/>
-      <c r="E6" s="11">
+      <c r="E6" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="11" t="n">
         <v>4.2</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="11" t="n">
         <v>2.6</v>
       </c>
-      <c r="H6" s="11">
-        <v>8.1999999999999993</v>
+      <c r="H6" s="11" t="n">
+        <v>8.2</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>55</v>
@@ -2098,17 +1869,17 @@
       <c r="K6" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="L6" s="11">
-        <v>2.2000000000000002</v>
+      <c r="L6" s="11" t="n">
+        <v>2.2</v>
       </c>
       <c r="M6" s="11"/>
-      <c r="N6" s="11">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="O6" s="11">
+      <c r="N6" s="11" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="O6" s="11" t="n">
         <v>180</v>
       </c>
-      <c r="P6" s="11">
+      <c r="P6" s="11" t="n">
         <v>1.5</v>
       </c>
       <c r="Q6" s="11"/>
@@ -2117,39 +1888,46 @@
       <c r="T6" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="O1" activeCellId="0" pane="topLeft" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125"/>
-    <col min="2" max="2" width="14.28515625"/>
-    <col min="3" max="3" width="13.7109375"/>
-    <col min="4" max="4" width="13.28515625"/>
-    <col min="5" max="5" width="13.7109375"/>
-    <col min="6" max="6" width="15.140625"/>
-    <col min="7" max="7" width="12.140625"/>
-    <col min="8" max="8" width="13.85546875"/>
-    <col min="9" max="9" width="12.42578125"/>
-    <col min="10" max="10" width="13.5703125"/>
-    <col min="11" max="11" width="13.42578125"/>
-    <col min="12" max="12" width="14.7109375"/>
-    <col min="13" max="13" width="13.42578125"/>
-    <col min="14" max="14" width="14.140625"/>
-    <col min="15" max="1025" width="8.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3411764705882"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7686274509804"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7686274509804"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2039215686275"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1921568627451"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.9098039215686"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.478431372549"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.6235294117647"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.4823529411765"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.7725490196078"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.4823529411765"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2191,72 +1969,81 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="2">
+      <c r="A2" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="13" t="n">
         <v>300</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="13" t="n">
         <v>1.8</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="13" t="n">
         <v>2.8</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="13" t="n">
         <v>1.7</v>
       </c>
       <c r="F2" s="11"/>
-      <c r="G2" s="13">
+      <c r="G2" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="13" t="n">
         <v>325</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="13" t="n">
         <v>400</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="13" t="n">
         <v>6000</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="13" t="n">
         <v>3.7</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="13" t="n">
         <v>270</v>
       </c>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125"/>
-    <col min="2" max="2" width="16.85546875"/>
-    <col min="3" max="3" width="16.42578125"/>
-    <col min="4" max="5" width="13.28515625"/>
-    <col min="6" max="6" width="15.85546875"/>
-    <col min="7" max="7" width="13.28515625"/>
-    <col min="8" max="8" width="14.7109375"/>
-    <col min="9" max="9" width="12.7109375"/>
-    <col min="10" max="10" width="12.140625"/>
-    <col min="11" max="11" width="14.140625"/>
-    <col min="12" max="1025" width="8.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9176470588235"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.7725490196078"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.7647058823529"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1921568627451"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>67</v>
@@ -2289,138 +2076,147 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+      <c r="A2" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="15" t="n">
         <v>37</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="15" t="n">
         <v>2400</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="16" t="n">
         <v>5.99</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="15" t="n">
         <v>2.99</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="17" t="n">
         <v>0.15</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="15" t="n">
         <v>5.13</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2" s="15" t="n">
         <v>2.94</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="15" t="n">
         <v>12</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2" s="15" t="n">
         <v>16</v>
       </c>
-      <c r="K2" s="15">
+      <c r="K2" s="15" t="n">
         <v>627</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+      <c r="A3" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="18" t="n">
         <v>37</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="18" t="n">
         <v>2400</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="18" t="n">
         <v>5.984</v>
       </c>
-      <c r="E3" s="18">
-        <v>2.9790000000000001</v>
-      </c>
-      <c r="F3" s="18">
+      <c r="E3" s="18" t="n">
+        <v>2.979</v>
+      </c>
+      <c r="F3" s="18" t="n">
         <v>0.3</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="18" t="n">
         <v>9.1</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="18" t="n">
         <v>5.2</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="18" t="n">
         <v>10</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="18" t="n">
         <v>20</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="18" t="n">
         <v>955</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+      <c r="A4" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="13" t="n">
         <v>37</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="13" t="n">
         <v>2400</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="13" t="n">
         <v>5.97</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="13" t="n">
         <v>2.99</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="13" t="n">
         <v>0.45</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="13" t="n">
         <v>11.78</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="13" t="n">
         <v>6.75</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="13" t="n">
         <v>32</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="13" t="n">
         <v>2090</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125"/>
-    <col min="2" max="2" width="16.85546875"/>
-    <col min="3" max="3" width="16.42578125"/>
-    <col min="4" max="5" width="13.28515625"/>
-    <col min="6" max="6" width="15.85546875"/>
-    <col min="7" max="7" width="13.28515625"/>
-    <col min="8" max="8" width="14.7109375"/>
-    <col min="9" max="9" width="12.85546875"/>
-    <col min="10" max="10" width="14.140625"/>
-    <col min="11" max="1025" width="8.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9176470588235"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.7725490196078"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.9058823529412"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>5</v>
@@ -2450,7 +2246,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -2462,7 +2258,7 @@
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -2474,7 +2270,7 @@
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -2487,33 +2283,40 @@
       <c r="J4" s="13"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E2" activeCellId="0" pane="topLeft" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125"/>
-    <col min="2" max="2" width="16.85546875"/>
-    <col min="3" max="3" width="16.42578125"/>
-    <col min="4" max="5" width="13.28515625"/>
-    <col min="6" max="6" width="15.85546875"/>
-    <col min="7" max="7" width="13.28515625"/>
-    <col min="8" max="10" width="14.7109375"/>
-    <col min="11" max="11" width="14.140625"/>
-    <col min="12" max="1025" width="8.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9176470588235"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="14.7725490196078"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>83</v>
@@ -2546,7 +2349,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -2559,7 +2362,7 @@
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -2572,7 +2375,7 @@
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -2586,38 +2389,45 @@
       <c r="K4" s="13"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="L6" activeCellId="0" pane="topLeft" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125"/>
-    <col min="2" max="2" width="16.85546875"/>
-    <col min="3" max="3" width="16.42578125"/>
-    <col min="4" max="4" width="15.42578125"/>
-    <col min="5" max="5" width="16.42578125"/>
-    <col min="6" max="6" width="13.7109375"/>
-    <col min="7" max="7" width="13.28515625"/>
-    <col min="8" max="8" width="12.140625"/>
-    <col min="9" max="9" width="18.85546875"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875"/>
-    <col min="13" max="13" width="14.140625"/>
-    <col min="14" max="1025" width="8.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4901960784314"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7686274509804"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1921568627451"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.9294117647059"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.356862745098"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.0705882352941"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.9137254901961"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2656,73 +2466,80 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="19">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
+      <c r="A2" s="19" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="19"/>
-      <c r="C2" s="19">
+      <c r="C2" s="19" t="n">
         <v>22.1</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="19" t="n">
         <v>217.5</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="19" t="n">
         <v>3.75</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="19" t="n">
         <v>4.74</v>
       </c>
-      <c r="G2" s="20">
+      <c r="G2" s="20" t="n">
         <v>1900</v>
       </c>
-      <c r="H2" s="20">
+      <c r="H2" s="20" t="n">
         <v>190</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2" s="20" t="n">
         <v>32</v>
       </c>
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
-      <c r="L2" s="21">
+      <c r="L2" s="21" t="n">
         <v>18400</v>
       </c>
       <c r="M2" s="22"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMI2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G1" activeCellId="0" pane="topLeft" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="23"/>
-    <col min="2" max="2" width="16.85546875" style="23"/>
-    <col min="3" max="3" width="16.42578125" style="23"/>
-    <col min="4" max="4" width="15.42578125" style="23"/>
-    <col min="5" max="5" width="19" style="23"/>
-    <col min="6" max="6" width="13.7109375" style="23"/>
-    <col min="7" max="7" width="13.28515625" style="23"/>
-    <col min="8" max="8" width="12.140625" style="23"/>
-    <col min="9" max="9" width="18.85546875" style="23"/>
-    <col min="10" max="10" width="14.5703125" style="23"/>
-    <col min="11" max="11" width="11.5703125" style="23"/>
-    <col min="12" max="12" width="14.85546875" style="23"/>
-    <col min="13" max="13" width="14.140625" style="23"/>
-    <col min="14" max="1023" width="8.7109375" style="23"/>
-    <col min="1024" max="1025" width="8.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="9.32156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="16.921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="16.4941176470588"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="15.4901960784314"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="19.0823529411765"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="13.7686274509804"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="23" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="23" width="12.1921568627451"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="23" width="18.9294117647059"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="23" width="14.6274509803922"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="23" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="23" width="14.9137254901961"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="23" width="14.2"/>
+    <col collapsed="false" hidden="false" max="1023" min="14" style="23" width="8.74901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="52.5" outlineLevel="0" r="1">
       <c r="A1" s="18"/>
       <c r="B1" s="2" t="s">
         <v>79</v>
@@ -2776,37 +2593,37 @@
       <c r="AA1" s="24"/>
       <c r="AB1" s="24"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
+      <c r="A2" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="12" t="n">
         <v>11.53</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="12" t="n">
         <v>65</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="26" t="n">
         <v>70</v>
       </c>
-      <c r="G2" s="26">
+      <c r="G2" s="26" t="n">
         <v>30</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="12" t="n">
         <v>393</v>
       </c>
-      <c r="I2" s="12">
+      <c r="I2" s="12" t="n">
         <v>250</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
-      <c r="L2" s="27">
+      <c r="L2" s="27" t="n">
         <v>240000</v>
       </c>
       <c r="M2" s="28"/>
@@ -2827,7 +2644,12 @@
       <c r="AB2" s="29"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>